<commit_message>
20230105 RENAME UI 코드
</commit_message>
<xml_diff>
--- a/ui 코드 설계.xlsx
+++ b/ui 코드 설계.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E2730F-9165-4A3A-9082-6B8D1CB32C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02372161-8601-4722-B1F6-68948CEB138D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5450" yWindow="2090" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="환자정보" sheetId="2" r:id="rId1"/>
@@ -57,20 +57,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Patlent_Birthdat_lineEdit
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>생년월일</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> Patlent_ChartNumber_lineEdit
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>차트번호</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -79,58 +69,30 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Gender_Male_pushButton</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>성별: Male 푸시버튼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Patlent_Gender_Female_pushButton, 
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Female  푸시버튼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Patlent_Gender_None_pushButton
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> None 푸시버튼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_FirstVist_dateEdit</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>첫 진료일</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_LastVist_dateEdit</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>마지막 진료일</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Mobile_lineEdit</t>
-  </si>
-  <si>
     <t>전화번호</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Phone_lineEdit</t>
-  </si>
-  <si>
     <t>휴대폰 번호</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -143,85 +105,39 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_DetailAddress_lineEdit</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>상세 주소</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Data_upper_openGLWidget</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>상악</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Data_lower_openGLWidget</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>하악</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Data_occlusion_openGLWidget</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>교합</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_New_pushButton</t>
-  </si>
-  <si>
     <t>New 버튼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Edit_pushButton</t>
-  </si>
-  <si>
     <t>Edit 버튼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_Delete_pushButton</t>
-  </si>
-  <si>
     <t>Delete 버튼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Patlent_comboBox</t>
-  </si>
-  <si>
     <t>이메일 콤보박스</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>PatlentlistView</t>
-  </si>
-  <si>
     <t xml:space="preserve">listView </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patlent_Name_lineEdit
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Patlent_Email_lineEdit
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Patlent_Address_lineEdit
-</t>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>2팀</t>
@@ -348,6 +264,97 @@
   </si>
   <si>
     <t>확대 이미지</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_Name_lineEdit
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_Birthdat_lineEdit
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_ChartNumber_lineEdit
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Gender_Male_pushButton</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_Gender_Female_pushButton, 
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_Gender_None_pushButton
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_FirstVist_dateEdit</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_LastVist_dateEdit</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Mobile_lineEdit</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Phone_lineEdit</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_Email_lineEdit
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_Address_lineEdit
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_DetailAddress_lineEdit</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Data_upper_openGLWidget</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Data_lower_openGLWidget</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Data_occlusion_openGLWidget</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_New_pushButton</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Edit_pushButton</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_Delete_pushButton</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_comboBox</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient_listView</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -1379,8 +1386,8 @@
   </sheetPr>
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -1394,7 +1401,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="45" customHeight="1">
@@ -1422,7 +1429,7 @@
     </row>
     <row r="5" spans="2:4" ht="35">
       <c r="B5" s="7" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>4</v>
@@ -1433,10 +1440,10 @@
     </row>
     <row r="6" spans="2:4" ht="35">
       <c r="B6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="12">
         <v>44931</v>
@@ -1444,10 +1451,10 @@
     </row>
     <row r="7" spans="2:4" ht="35">
       <c r="B7" s="10" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="12">
         <v>44931</v>
@@ -1455,10 +1462,10 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="12">
         <v>44931</v>
@@ -1466,10 +1473,10 @@
     </row>
     <row r="9" spans="2:4" ht="35">
       <c r="B9" s="10" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" s="12">
         <v>44931</v>
@@ -1477,10 +1484,10 @@
     </row>
     <row r="10" spans="2:4" ht="35">
       <c r="B10" s="10" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D10" s="12">
         <v>44931</v>
@@ -1488,10 +1495,10 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="13" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D11" s="12">
         <v>44931</v>
@@ -1499,10 +1506,10 @@
     </row>
     <row r="12" spans="2:4" ht="17.5">
       <c r="B12" s="10" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D12" s="12">
         <v>44931</v>
@@ -1510,10 +1517,10 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="13" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D13" s="12">
         <v>44931</v>
@@ -1521,10 +1528,10 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="13" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D14" s="12">
         <v>44931</v>
@@ -1532,10 +1539,10 @@
     </row>
     <row r="15" spans="2:4" ht="18" customHeight="1">
       <c r="B15" s="10" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D15" s="12">
         <v>44931</v>
@@ -1543,10 +1550,10 @@
     </row>
     <row r="16" spans="2:4" ht="20" customHeight="1">
       <c r="B16" s="10" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D16" s="12">
         <v>44931</v>
@@ -1554,10 +1561,10 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="13" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D17" s="12">
         <v>44931</v>
@@ -1565,10 +1572,10 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="13" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D18" s="12">
         <v>44931</v>
@@ -1576,10 +1583,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="13" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D19" s="12">
         <v>44931</v>
@@ -1587,10 +1594,10 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="13" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D20" s="12">
         <v>44931</v>
@@ -1598,10 +1605,10 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="13" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D21" s="12">
         <v>44931</v>
@@ -1609,10 +1616,10 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="13" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D22" s="12">
         <v>44931</v>
@@ -1620,10 +1627,10 @@
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="13" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D23" s="12">
         <v>44931</v>
@@ -1631,10 +1638,10 @@
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="13" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D24" s="12">
         <v>44931</v>
@@ -1642,10 +1649,10 @@
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="14" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D25" s="16">
         <v>44931</v>
@@ -1696,7 +1703,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="45" customHeight="1">
@@ -1713,7 +1720,7 @@
     </row>
     <row r="4" spans="2:4" ht="30" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -1724,10 +1731,10 @@
     </row>
     <row r="5" spans="2:4" ht="17.5">
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9">
         <v>44931</v>
@@ -1735,10 +1742,10 @@
     </row>
     <row r="6" spans="2:4" ht="16.5" customHeight="1">
       <c r="B6" s="10" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="12">
         <v>44931</v>
@@ -1746,10 +1753,10 @@
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D7" s="12">
         <v>44931</v>
@@ -1757,10 +1764,10 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D8" s="12">
         <v>44931</v>
@@ -1768,10 +1775,10 @@
     </row>
     <row r="9" spans="2:4" ht="17.5" customHeight="1">
       <c r="B9" s="10" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D9" s="12">
         <v>44931</v>
@@ -1779,10 +1786,10 @@
     </row>
     <row r="10" spans="2:4" ht="21.5" customHeight="1">
       <c r="B10" s="10" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D10" s="12">
         <v>44931</v>
@@ -1790,10 +1797,10 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="13" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D11" s="12">
         <v>44931</v>
@@ -1801,10 +1808,10 @@
     </row>
     <row r="12" spans="2:4" ht="17.5">
       <c r="B12" s="10" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D12" s="12">
         <v>44931</v>
@@ -1812,10 +1819,10 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="13" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="D13" s="12">
         <v>44931</v>
@@ -1823,10 +1830,10 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="14" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D14" s="16">
         <v>44931</v>
@@ -1879,7 +1886,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="33.75" customHeight="1">
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="45" customHeight="1">
@@ -1896,7 +1903,7 @@
     </row>
     <row r="4" spans="2:4" ht="30" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -1907,10 +1914,10 @@
     </row>
     <row r="5" spans="2:4" ht="17.5">
       <c r="B5" s="7" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D5" s="9">
         <v>44931</v>
@@ -1918,10 +1925,10 @@
     </row>
     <row r="6" spans="2:4" ht="16.5" customHeight="1">
       <c r="B6" s="10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D6" s="12">
         <v>44931</v>
@@ -1929,10 +1936,10 @@
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D7" s="12">
         <v>44931</v>
@@ -1940,10 +1947,10 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D8" s="12">
         <v>44931</v>
@@ -1951,10 +1958,10 @@
     </row>
     <row r="9" spans="2:4" ht="17.5" customHeight="1">
       <c r="B9" s="10" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D9" s="12">
         <v>44931</v>
@@ -1962,10 +1969,10 @@
     </row>
     <row r="10" spans="2:4" ht="21.5" customHeight="1">
       <c r="B10" s="10" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D10" s="12">
         <v>44931</v>
@@ -1973,10 +1980,10 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="14" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D11" s="16">
         <v>44931</v>

</xml_diff>

<commit_message>
20230106 RENAME UI 코드
</commit_message>
<xml_diff>
--- a/ui 코드 설계.xlsx
+++ b/ui 코드 설계.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C94B887-909B-4F2F-A589-B098A297863B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB01332-39B7-4F26-9D17-D2A58B51FF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4390" yWindow="780" windowWidth="19200" windowHeight="11260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>완료 날짜</t>
   </si>
@@ -249,9 +249,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>첫번째 단어는 대문자로 시작하고 (언더스코프)로 단어들 사이를 구분한다.</t>
-  </si>
-  <si>
     <t>3D Modelview 확대 이미지 UI</t>
   </si>
   <si>
@@ -378,6 +375,14 @@
   </si>
   <si>
     <t>viewExpansionSavepushButton</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>카멜표기법 으로 구분한다.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>카멜표기법 으로 구분한다.</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -1409,8 +1414,8 @@
   </sheetPr>
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -1434,7 +1439,7 @@
     </row>
     <row r="3" spans="2:4" ht="49.5" customHeight="1">
       <c r="B3" s="17" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1551,7 +1556,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>13</v>
@@ -1562,7 +1567,7 @@
     </row>
     <row r="15" spans="2:4" ht="18" customHeight="1">
       <c r="B15" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>14</v>
@@ -1573,7 +1578,7 @@
     </row>
     <row r="16" spans="2:4" ht="20" customHeight="1">
       <c r="B16" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>15</v>
@@ -1584,7 +1589,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>16</v>
@@ -1595,7 +1600,7 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>17</v>
@@ -1606,7 +1611,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>18</v>
@@ -1617,7 +1622,7 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>19</v>
@@ -1628,7 +1633,7 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>20</v>
@@ -1639,7 +1644,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>21</v>
@@ -1650,7 +1655,7 @@
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>22</v>
@@ -1661,7 +1666,7 @@
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>23</v>
@@ -1672,7 +1677,7 @@
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>24</v>
@@ -1712,7 +1717,7 @@
   <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -1736,7 +1741,7 @@
     </row>
     <row r="3" spans="2:4" ht="49.5" customHeight="1">
       <c r="B3" s="17" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1754,7 +1759,7 @@
     </row>
     <row r="5" spans="2:4" ht="17.5">
       <c r="B5" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>26</v>
@@ -1765,7 +1770,7 @@
     </row>
     <row r="6" spans="2:4" ht="16.5" customHeight="1">
       <c r="B6" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>6</v>
@@ -1776,7 +1781,7 @@
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>27</v>
@@ -1787,7 +1792,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>28</v>
@@ -1798,7 +1803,7 @@
     </row>
     <row r="9" spans="2:4" ht="17.5" customHeight="1">
       <c r="B9" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>29</v>
@@ -1809,7 +1814,7 @@
     </row>
     <row r="10" spans="2:4" ht="21.5" customHeight="1">
       <c r="B10" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>30</v>
@@ -1820,7 +1825,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>31</v>
@@ -1831,7 +1836,7 @@
     </row>
     <row r="12" spans="2:4" ht="17.5">
       <c r="B12" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>32</v>
@@ -1842,7 +1847,7 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>33</v>
@@ -1853,7 +1858,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>34</v>
@@ -1895,7 +1900,7 @@
   <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -1919,14 +1924,14 @@
     </row>
     <row r="3" spans="2:4" ht="49.5" customHeight="1">
       <c r="B3" s="17" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" ht="30" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
@@ -1937,7 +1942,7 @@
     </row>
     <row r="5" spans="2:4" ht="17.5">
       <c r="B5" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>35</v>
@@ -1948,7 +1953,7 @@
     </row>
     <row r="6" spans="2:4" ht="16.5" customHeight="1">
       <c r="B6" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>36</v>
@@ -1959,7 +1964,7 @@
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>37</v>
@@ -1970,7 +1975,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>38</v>
@@ -1981,7 +1986,7 @@
     </row>
     <row r="9" spans="2:4" ht="17.5" customHeight="1">
       <c r="B9" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>39</v>
@@ -1992,7 +1997,7 @@
     </row>
     <row r="10" spans="2:4" ht="21.5" customHeight="1">
       <c r="B10" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>40</v>
@@ -2003,7 +2008,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>41</v>
@@ -2014,10 +2019,10 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="16">
         <v>44931</v>
@@ -2068,15 +2073,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2376,6 +2372,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B3E0A64-3B79-40D0-B5B8-9F6FE2202932}">
   <ds:schemaRefs>
@@ -2389,14 +2394,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4994F8E-3141-47F3-91B7-8A348AFEAE97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A16C7A7-3246-4EB4-B7D0-9FB37D6AB99A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2417,6 +2414,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4994F8E-3141-47F3-91B7-8A348AFEAE97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>